<commit_message>
collection scripts now adapted for parallelization
</commit_message>
<xml_diff>
--- a/data/data_digitization/collection_data/1_raw_data/HJ-7-coll-entry.xlsx
+++ b/data/data_digitization/collection_data/1_raw_data/HJ-7-coll-entry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emma/Desktop/LDP Internship/Harvey_Janszen_Legacy_Project/data/data_digitization/collection_data/1_raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF73100-7700-6048-A0FA-1E8431B2F008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7D8401-E8A7-C84B-A5B0-5DFF622C5540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19560" xr2:uid="{6CD260D0-3248-EC4C-A246-EE521030FA00}"/>
   </bookViews>
@@ -2133,7 +2133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="189">
   <si>
     <t>habitat</t>
   </si>
@@ -2688,6 +2688,18 @@
   </si>
   <si>
     <t>North Pender Island; Magic Lake; fen below lake</t>
+  </si>
+  <si>
+    <t>Matthiola incana</t>
+  </si>
+  <si>
+    <t>Polygonum aviculare</t>
+  </si>
+  <si>
+    <t>Actea rubra</t>
+  </si>
+  <si>
+    <t>Actaea rubra</t>
   </si>
 </sst>
 </file>
@@ -3160,12 +3172,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E2B542-A597-DF4D-A726-D9C00BB4087B}">
-  <dimension ref="A1:AF115"/>
+  <dimension ref="A1:AF119"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="206" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="206" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8195,6 +8207,182 @@
         <v>169</v>
       </c>
     </row>
+    <row r="116" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>16</v>
+      </c>
+      <c r="B116" s="3">
+        <v>1</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2043</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H116" s="3">
+        <v>19810716</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K116" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L116" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M116" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q116" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>16</v>
+      </c>
+      <c r="B117" s="3">
+        <v>2</v>
+      </c>
+      <c r="C117" s="3">
+        <v>2044</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="H117" s="3">
+        <v>19810716</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J117" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K117" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L117" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M117" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q117" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>16</v>
+      </c>
+      <c r="B118" s="3">
+        <v>3</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2045</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F118" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H118" s="3">
+        <v>19810716</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J118" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K118" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L118" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M118" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q118" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" ht="102" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>16</v>
+      </c>
+      <c r="B119" s="3">
+        <v>4</v>
+      </c>
+      <c r="C119" s="3">
+        <v>2046</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H119" s="3">
+        <v>19810716</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K119" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L119" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M119" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q119" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>